<commit_message>
left Forcasting half finished
</commit_message>
<xml_diff>
--- a/ML/ML_ready/first_try.xlsx
+++ b/ML/ML_ready/first_try.xlsx
@@ -636,160 +636,160 @@
         </is>
       </c>
       <c r="B2">
-        <v>11761868</v>
+        <v>811759</v>
       </c>
       <c r="C2">
-        <v>12597812.949</v>
+        <v>835944.9489999991</v>
       </c>
       <c r="D2">
-        <v>13557538</v>
+        <v>959725.0510000009</v>
       </c>
       <c r="E2">
         <v>849626.801</v>
       </c>
       <c r="F2">
-        <v>1591239.716</v>
+        <v>741612.915</v>
       </c>
       <c r="G2">
-        <v>2752321</v>
+        <v>1161081.284</v>
       </c>
       <c r="H2">
-        <v>4886117</v>
+        <v>2133796</v>
       </c>
       <c r="I2">
-        <v>7862614.263</v>
+        <v>2976497.263</v>
       </c>
       <c r="J2">
-        <v>9946502</v>
+        <v>2134978.462</v>
       </c>
       <c r="K2">
-        <v>11309389</v>
+        <v>1362887</v>
       </c>
       <c r="M2">
         <v>13190179</v>
       </c>
       <c r="N2">
-        <v>14410923</v>
+        <v>1220744</v>
       </c>
       <c r="O2">
-        <v>15657751</v>
+        <v>1246828</v>
       </c>
       <c r="P2">
-        <v>16677584</v>
+        <v>1019833</v>
       </c>
       <c r="Q2">
         <v>1001582</v>
       </c>
       <c r="R2">
-        <v>2206519</v>
+        <v>1204937</v>
       </c>
       <c r="S2">
-        <v>4032494.33</v>
+        <v>1825975.33</v>
       </c>
       <c r="T2">
-        <v>6564038</v>
+        <v>2531543.67</v>
       </c>
       <c r="U2">
-        <v>9724991</v>
+        <v>3160953</v>
       </c>
       <c r="V2">
-        <v>12545411.586</v>
+        <v>2820420.585999999</v>
       </c>
       <c r="W2">
-        <v>14639900.324</v>
+        <v>2094488.738</v>
       </c>
       <c r="X2">
-        <v>15872348</v>
+        <v>1232448</v>
       </c>
       <c r="Y2">
-        <v>16870241</v>
+        <v>997893</v>
       </c>
       <c r="Z2">
-        <v>17892075.94</v>
+        <v>1021834.940000001</v>
       </c>
       <c r="AA2">
-        <v>19117885.711</v>
+        <v>1225809.770999998</v>
       </c>
       <c r="AB2">
-        <v>20199861</v>
+        <v>1081975.289000001</v>
       </c>
       <c r="AC2">
         <v>1011785</v>
       </c>
       <c r="AD2">
-        <v>1912646</v>
+        <v>900861</v>
       </c>
       <c r="AE2">
-        <v>3413294</v>
+        <v>1500648</v>
       </c>
       <c r="AF2">
-        <v>5927589</v>
+        <v>2514295</v>
       </c>
       <c r="AG2">
-        <v>9420653</v>
+        <v>3493064</v>
       </c>
       <c r="AH2">
-        <v>11689872</v>
+        <v>2269219</v>
       </c>
       <c r="AI2">
-        <v>13288686.403</v>
+        <v>1598814.403000001</v>
       </c>
       <c r="AJ2">
-        <v>14429096</v>
+        <v>1140410</v>
       </c>
       <c r="AK2">
-        <v>15239330</v>
+        <v>810234</v>
       </c>
       <c r="AL2">
-        <v>16459047</v>
+        <v>1219717</v>
       </c>
       <c r="AM2">
-        <v>17558287</v>
+        <v>1099240</v>
       </c>
       <c r="AN2">
-        <v>18673339</v>
+        <v>1115052</v>
       </c>
       <c r="AO2">
         <v>1003393</v>
       </c>
       <c r="AP2">
-        <v>1961342</v>
+        <v>957949</v>
       </c>
       <c r="AQ2">
-        <v>3992789</v>
+        <v>2031447</v>
       </c>
       <c r="AR2">
-        <v>6947863</v>
+        <v>2955074</v>
       </c>
       <c r="AS2">
-        <v>10499775</v>
+        <v>3551912</v>
       </c>
       <c r="AT2">
-        <v>13725941.652</v>
+        <v>3226166.652000001</v>
       </c>
       <c r="AU2">
-        <v>15606270</v>
+        <v>1880328</v>
       </c>
       <c r="AV2">
-        <v>16996524</v>
+        <v>1390254</v>
       </c>
       <c r="AW2">
-        <v>17960932</v>
+        <v>964408</v>
       </c>
       <c r="AX2">
-        <v>19144129</v>
+        <v>1183197</v>
       </c>
       <c r="AY2">
-        <v>20676475</v>
+        <v>1532346</v>
       </c>
       <c r="AZ2">
-        <v>22011562</v>
+        <v>1335087</v>
       </c>
       <c r="BA2">
         <v>1149309</v>
       </c>
       <c r="BB2">
-        <v>2170630</v>
+        <v>1021321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>